<commit_message>
5,6 자료실 outlier 제거
</commit_message>
<xml_diff>
--- a/static/5자료실.xlsx
+++ b/static/5자료실.xlsx
@@ -2175,7 +2175,7 @@
   <dimension ref="A1:AA100"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U11" activeCellId="0" sqref="U11"/>
+      <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2516,7 +2516,7 @@
         <v>668.9</v>
       </c>
       <c r="F7" s="1" t="n">
-        <v>68.9</v>
+        <v>668.9</v>
       </c>
       <c r="G7" s="1" t="n">
         <v>669</v>
@@ -4761,7 +4761,7 @@
         <v>646.3</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>464.01</v>
+        <v>646.01</v>
       </c>
       <c r="D53" s="1" t="n">
         <v>643</v>
@@ -5058,7 +5058,7 @@
         <v>631.4951</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>531.53</v>
+        <v>631.53</v>
       </c>
       <c r="E59" s="1" t="n">
         <v>631.7</v>

</xml_diff>